<commit_message>
add email filed for imapsvr
</commit_message>
<xml_diff>
--- a/public/upload/files/email_example.xlsx
+++ b/public/upload/files/email_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voke\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phpstudy_pro\WWW\all-mail.im\public\upload\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A95D01-DCF8-43C0-BFD2-0DB3AD0FE45D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E4F2B4-44BD-431F-9B40-ACD23300D03F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2676" yWindow="816" windowWidth="20364" windowHeight="11544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>email_name</t>
   </si>
@@ -50,6 +50,12 @@
   <si>
     <t>djeimibrainina1989@rambler.ru</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>imapsvr</t>
+  </si>
+  <si>
+    <t>imap.rambler.ru</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -421,7 +427,7 @@
     <col min="4" max="4" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
+    <row r="1" spans="1:5" ht="21" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,13 +435,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -443,9 +452,12 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>